<commit_message>
refs #459, Revisions - Import Revisions to Existing Orders and Push; fixed revised IO uploading (now referenced by order_id rather then order's name
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_revised.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_revised.xlsx
@@ -24,16 +24,19 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -134,7 +137,7 @@
     <t>Order Name:</t>
   </si>
   <si>
-    <t>Otterbein University on Audience Network &amp; RR (6.27-8.18.13) – 799361</t>
+    <t>Otterbein University on Audience Network &amp; RR (6.27-8.18.13) – 799361 Revised</t>
   </si>
   <si>
     <t>Company Address:</t>
@@ -1452,7 +1455,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1522,15 +1525,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>498240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1545,8 +1548,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="183240"/>
-          <a:ext cx="1229760" cy="598320"/>
+          <a:off x="266760" y="174240"/>
+          <a:ext cx="1229400" cy="597960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1558,15 +1561,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>37800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1575,8 +1578,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="21600"/>
-          <a:ext cx="12353760" cy="45720"/>
+          <a:off x="162000" y="12600"/>
+          <a:ext cx="12353400" cy="45360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1597,15 +1600,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>37800</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1614,8 +1617,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="850320"/>
-          <a:ext cx="12353760" cy="45720"/>
+          <a:off x="162000" y="841320"/>
+          <a:ext cx="12353400" cy="45360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1636,15 +1639,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>49320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1653,8 +1656,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="6182280"/>
-          <a:ext cx="12391920" cy="141120"/>
+          <a:off x="162000" y="6173280"/>
+          <a:ext cx="12391560" cy="140760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1675,15 +1678,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>39960</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1692,8 +1695,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="2936160"/>
-          <a:ext cx="12382560" cy="43920"/>
+          <a:off x="162000" y="2927160"/>
+          <a:ext cx="12382200" cy="43560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1719,15 +1722,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>192240</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
+      <xdr:colOff>283680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>201240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1742,8 +1745,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="192240" y="12240"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="219240" y="3240"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1760,15 +1763,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>267840</xdr:rowOff>
+      <xdr:rowOff>258480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1783,8 +1786,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="69480"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="266760" y="60480"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1801,15 +1804,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>219960</xdr:rowOff>
+      <xdr:rowOff>210600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1824,8 +1827,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="21600"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="266760" y="12600"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1845,7 +1848,7 @@
   <dimension ref="A1:AI181"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F29" activeCellId="0" pane="topLeft" sqref="F29"/>
+      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
refs #459, Revisions - Import Revisions to Existing Orders and Push; fixed revised assets storing
Conflicts:
	app/controllers/orders_controller.rb
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_revised.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_revised.xlsx
@@ -25,18 +25,21 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -71,13 +74,13 @@
     </r>
   </si>
   <si>
-    <t>Alexandra Piechota</t>
+    <t>Travis</t>
   </si>
   <si>
     <t>Trafficking Contact:</t>
   </si>
   <si>
-    <t>Ronnie Wallace</t>
+    <t>Amol Brid</t>
   </si>
   <si>
     <t>Phone:</t>
@@ -113,13 +116,13 @@
     <t>Media Contact:</t>
   </si>
   <si>
-    <t>Mary Ball</t>
+    <t>Mary Corner</t>
   </si>
   <si>
     <t>Billing Contact:</t>
   </si>
   <si>
-    <t>Bryan Snyder</t>
+    <t>Amber Smith</t>
   </si>
   <si>
     <t>Advertiser Name:</t>
@@ -1455,7 +1458,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1525,15 +1528,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1548,8 +1551,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="174240"/>
-          <a:ext cx="1229400" cy="597960"/>
+          <a:off x="293760" y="165240"/>
+          <a:ext cx="1229040" cy="597600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1561,15 +1564,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>37800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1578,8 +1581,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="12600"/>
-          <a:ext cx="12353400" cy="45360"/>
+          <a:off x="189000" y="3600"/>
+          <a:ext cx="12353040" cy="45000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1600,15 +1603,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>37800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1617,8 +1620,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="841320"/>
-          <a:ext cx="12353400" cy="45360"/>
+          <a:off x="189000" y="832320"/>
+          <a:ext cx="12353040" cy="45000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1639,15 +1642,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1656,8 +1659,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="6173280"/>
-          <a:ext cx="12391560" cy="140760"/>
+          <a:off x="189000" y="6164280"/>
+          <a:ext cx="12391200" cy="140400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1678,15 +1681,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
+      <xdr:colOff>93240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1695,8 +1698,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="2927160"/>
-          <a:ext cx="12382200" cy="43560"/>
+          <a:off x="189000" y="2918160"/>
+          <a:ext cx="12381840" cy="43200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1722,15 +1725,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>283680</xdr:colOff>
+      <xdr:colOff>310320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>201240</xdr:rowOff>
+      <xdr:rowOff>200880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1745,8 +1748,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="219240" y="3240"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="246240" y="3240"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1763,15 +1766,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>357840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>249120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1786,8 +1789,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="60480"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="293760" y="51480"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1804,15 +1807,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>357840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>201240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1827,8 +1830,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="12600"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="293760" y="3600"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1848,7 +1851,7 @@
   <dimension ref="A1:AI181"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
+      <selection activeCell="E13" activeCellId="0" pane="topLeft" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>